<commit_message>
Add sell nothing to the grid test to spreadsheet
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/run/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/run/synfuels_model_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7FEF7E9-96AF-47C2-9005-9E053A283F3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3049DB-1285-437D-BCD8-094B94339089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Capacity_Market" sheetId="3" r:id="rId3"/>
     <sheet name="Transfer_rates" sheetId="4" r:id="rId4"/>
     <sheet name="grid_sellall_test" sheetId="5" r:id="rId5"/>
+    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="94">
   <si>
     <t>Source</t>
   </si>
@@ -315,6 +316,12 @@
   </si>
   <si>
     <t>Optimized capacity</t>
+  </si>
+  <si>
+    <t>Should sell as little as possible to grid</t>
+  </si>
+  <si>
+    <t>Still smallest possible since constant prices everywhere</t>
   </si>
 </sst>
 </file>
@@ -1335,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD4092A-9167-4B1E-A144-D4BB7A88B529}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection sqref="A1:F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1583,4 +1590,263 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
+  <dimension ref="A1:E22"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="31.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B1">
+        <v>0.1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <f>B1/1000</f>
+        <v>1E-4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B3" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C3" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>71</v>
+      </c>
+      <c r="B5" s="3">
+        <v>10000</v>
+      </c>
+      <c r="C5" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
+        <v>28</v>
+      </c>
+      <c r="E8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C9" s="3">
+        <v>750000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>73</v>
+      </c>
+      <c r="E9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="3">
+        <v>-750000</v>
+      </c>
+      <c r="C10" s="3">
+        <v>-1000</v>
+      </c>
+      <c r="D10" t="s">
+        <v>73</v>
+      </c>
+      <c r="E10" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11" s="3">
+        <v>-100000</v>
+      </c>
+      <c r="C11" s="3">
+        <v>-1000</v>
+      </c>
+      <c r="D11" t="s">
+        <v>75</v>
+      </c>
+      <c r="E11" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C12" s="3">
+        <v>500000</v>
+      </c>
+      <c r="D12" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>16</v>
+      </c>
+      <c r="B13" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C13" s="3">
+        <v>200000</v>
+      </c>
+      <c r="D13" t="s">
+        <v>88</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>91</v>
+      </c>
+      <c r="C17" t="s">
+        <v>28</v>
+      </c>
+      <c r="D17" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="3">
+        <v>-750000</v>
+      </c>
+      <c r="C19" t="s">
+        <v>73</v>
+      </c>
+      <c r="D19" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="3">
+        <v>-100000</v>
+      </c>
+      <c r="C20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D20" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>16</v>
+      </c>
+      <c r="B22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C22" t="s">
+        <v>88</v>
+      </c>
+      <c r="D22" t="s">
+        <v>64</v>
+      </c>
+      <c r="E22" t="s">
+        <v>93</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Write tests to check results consistency with defined market prices
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/run/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/run/synfuels_model_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\run\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA3049DB-1285-437D-BCD8-094B94339089}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4C28C23-901D-4826-A074-3F0F659E60E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="5" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="38355" yWindow="7725" windowWidth="14400" windowHeight="7365" activeTab="5" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="94">
   <si>
     <t>Source</t>
   </si>
@@ -359,11 +359,11 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -686,12 +686,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="2"/>
+    <col min="1" max="1" width="8.7265625" style="1"/>
     <col min="2" max="2" width="85.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B1" t="s">
@@ -702,10 +702,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1"/>
+      <c r="B2" s="3"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -720,7 +720,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
       <c r="B3" t="s">
@@ -740,7 +740,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
@@ -760,7 +760,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
       <c r="B5" t="s">
@@ -780,7 +780,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B6" t="s">
@@ -803,7 +803,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B7" t="s">
@@ -814,7 +814,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
       <c r="B8" t="s">
@@ -1115,15 +1115,15 @@
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-      <c r="G2" s="1"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1135,14 +1135,14 @@
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="3">
+      <c r="D3" s="2">
         <f>B3*1000/(24*3600)</f>
         <v>18.287037037037038</v>
       </c>
       <c r="E3" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="2">
         <f>B3*1000/24</f>
         <v>65833.333333333328</v>
       </c>
@@ -1160,14 +1160,14 @@
       <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="3">
+      <c r="D4" s="2">
         <f>B4*1000/(24*3600)</f>
         <v>2.9513888888888888</v>
       </c>
       <c r="E4" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="3">
+      <c r="F4" s="2">
         <f>B4*1000/24</f>
         <v>10625</v>
       </c>
@@ -1185,13 +1185,13 @@
       <c r="C5" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="3">
+      <c r="D5" s="2">
         <v>14900</v>
       </c>
       <c r="E5" t="s">
         <v>73</v>
       </c>
-      <c r="F5" s="3">
+      <c r="F5" s="2">
         <v>14900</v>
       </c>
       <c r="G5" t="s">
@@ -1199,15 +1199,15 @@
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A6" s="1" t="s">
+      <c r="A6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1219,14 +1219,14 @@
       <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <f>B7*1000/(24*3600)</f>
         <v>2.0370370370370372</v>
       </c>
       <c r="E7" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="3">
+      <c r="F7" s="2">
         <f>B7*1000/24</f>
         <v>7333.333333333333</v>
       </c>
@@ -1244,14 +1244,14 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <f t="shared" ref="D8:D9" si="0">B8*1000/(24*3600)</f>
         <v>2.4652777777777777</v>
       </c>
       <c r="E8" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="2">
         <f t="shared" ref="F8:F9" si="1">B8*1000/24</f>
         <v>8875</v>
       </c>
@@ -1269,14 +1269,14 @@
       <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <f t="shared" si="0"/>
         <v>1.3657407407407407</v>
       </c>
       <c r="E9" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="2">
         <f t="shared" si="1"/>
         <v>4916.666666666667</v>
       </c>
@@ -1290,11 +1290,11 @@
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A12" s="1" t="s">
+      <c r="A12" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1308,11 +1308,11 @@
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A14" s="1" t="s">
+      <c r="A14" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -1342,8 +1342,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD4092A-9167-4B1E-A144-D4BB7A88B529}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection sqref="A1:F22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1375,7 +1375,7 @@
       <c r="A3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>1E-4</v>
       </c>
       <c r="C3" t="s">
@@ -1386,7 +1386,7 @@
       <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>1E-4</v>
       </c>
       <c r="C4" t="s">
@@ -1397,7 +1397,7 @@
       <c r="A5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>1E-4</v>
       </c>
       <c r="C5" t="s">
@@ -1430,10 +1430,10 @@
       <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>1000</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>750000</v>
       </c>
       <c r="D9" t="s">
@@ -1447,10 +1447,10 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>-750000</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>-1000</v>
       </c>
       <c r="D10" t="s">
@@ -1464,10 +1464,10 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>-100000</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>-1000</v>
       </c>
       <c r="D11" t="s">
@@ -1481,10 +1481,10 @@
       <c r="A12" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>1000</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>500000</v>
       </c>
       <c r="D12" t="s">
@@ -1498,10 +1498,10 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>1000</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>200000</v>
       </c>
       <c r="D13" t="s">
@@ -1544,7 +1544,7 @@
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>-1000</v>
       </c>
       <c r="C19" t="s">
@@ -1558,7 +1558,7 @@
       <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>-1000</v>
       </c>
       <c r="C20" t="s">
@@ -1577,7 +1577,7 @@
       <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1000</v>
       </c>
       <c r="C22" t="s">
@@ -1596,8 +1596,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1631,7 +1631,7 @@
       <c r="A3" t="s">
         <v>69</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>10000</v>
       </c>
       <c r="C3" t="s">
@@ -1642,7 +1642,7 @@
       <c r="A4" t="s">
         <v>70</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>10000</v>
       </c>
       <c r="C4" t="s">
@@ -1653,7 +1653,7 @@
       <c r="A5" t="s">
         <v>71</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>10000</v>
       </c>
       <c r="C5" t="s">
@@ -1686,10 +1686,10 @@
       <c r="A9" t="s">
         <v>84</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>1000</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>750000</v>
       </c>
       <c r="D9" t="s">
@@ -1703,10 +1703,10 @@
       <c r="A10" t="s">
         <v>17</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>-750000</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>-1000</v>
       </c>
       <c r="D10" t="s">
@@ -1720,10 +1720,10 @@
       <c r="A11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>-100000</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>-1000</v>
       </c>
       <c r="D11" t="s">
@@ -1737,10 +1737,10 @@
       <c r="A12" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="2">
         <v>1000</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>500000</v>
       </c>
       <c r="D12" t="s">
@@ -1754,10 +1754,10 @@
       <c r="A13" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="2">
         <v>1000</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>200000</v>
       </c>
       <c r="D13" t="s">
@@ -1795,12 +1795,21 @@
       <c r="A18" t="s">
         <v>84</v>
       </c>
+      <c r="B18" s="2">
+        <v>750000</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="2">
         <v>-750000</v>
       </c>
       <c r="C19" t="s">
@@ -1814,7 +1823,7 @@
       <c r="A20" t="s">
         <v>15</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="2">
         <v>-100000</v>
       </c>
       <c r="C20" t="s">
@@ -1833,7 +1842,7 @@
       <c r="A22" t="s">
         <v>16</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="2">
         <v>1000</v>
       </c>
       <c r="C22" t="s">

</xml_diff>